<commit_message>
added timmer for delay requests"
</commit_message>
<xml_diff>
--- a/samples/syn_add.xlsx
+++ b/samples/syn_add.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamalakar.adepu\Desktop\bolt-tech\node-express-mvc-master\newrelic-utility-tool\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62184EC-4592-440B-BD3E-90C94D7DEAAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C575C92F-EB20-4CF0-BD35-E2BC0367D47E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{4C83127D-4EF5-4C9F-9CBD-DB09973DD4C8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="39">
   <si>
     <t>name</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>AWS_AP_SOUTH_1</t>
-  </si>
-  <si>
-    <t>browser</t>
   </si>
   <si>
     <t>enabled</t>
@@ -112,6 +109,54 @@
   </si>
   <si>
     <t>monitor_scripting_monitirng</t>
+  </si>
+  <si>
+    <t>monitor112</t>
+  </si>
+  <si>
+    <t>monitor_testing_new12</t>
+  </si>
+  <si>
+    <t>monitorvv</t>
+  </si>
+  <si>
+    <t>monitorvv1</t>
+  </si>
+  <si>
+    <t>monitorvv2</t>
+  </si>
+  <si>
+    <t>monitorvv3</t>
+  </si>
+  <si>
+    <t>monitorvv4</t>
+  </si>
+  <si>
+    <t>monitor1x</t>
+  </si>
+  <si>
+    <t>monitor_testing_newx</t>
+  </si>
+  <si>
+    <t>monitor1xx</t>
+  </si>
+  <si>
+    <t>monitor_testing_newxx</t>
+  </si>
+  <si>
+    <t>monitor1xx1</t>
+  </si>
+  <si>
+    <t>monitor_testing_newxx1</t>
+  </si>
+  <si>
+    <t>monitor1xx22</t>
+  </si>
+  <si>
+    <t>monitor_testing_newxx12</t>
+  </si>
+  <si>
+    <t>browser</t>
   </si>
 </sst>
 </file>
@@ -539,14 +584,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32280B03-C193-499E-BFCF-20CA7D91CECC}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" customWidth="1"/>
@@ -579,19 +625,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="L1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -608,10 +654,10 @@
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="4">
         <v>0.1</v>
@@ -627,9 +673,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4">
         <v>15</v>
@@ -641,10 +687,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="4">
         <v>0.1</v>
@@ -662,7 +708,7 @@
     </row>
     <row r="4" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="4">
         <v>15</v>
@@ -674,10 +720,10 @@
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="4">
         <v>0.1</v>
@@ -693,12 +739,12 @@
         <v>0</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4">
         <v>15</v>
@@ -710,10 +756,10 @@
         <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="4">
         <v>0.1</v>
@@ -729,7 +775,517 @@
         <v>0</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="4">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="4">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="4">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="4">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="4">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="4">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="4">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="4">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="4">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="4">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="4">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>